<commit_message>
updated data dictionary and model
</commit_message>
<xml_diff>
--- a/data-dictionary.xlsx
+++ b/data-dictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>billing_acct_id</t>
   </si>
@@ -90,10 +90,88 @@
     <t>email, may be blank if NA.</t>
   </si>
   <si>
-    <t>marketing lead source (level 1 depth, ex. "radio")</t>
-  </si>
-  <si>
-    <t>marketing lead source (level 2 depth, ex. "radio for discounted tune-up in 2017")</t>
+    <t>call_type</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>taken_date</t>
+  </si>
+  <si>
+    <t>job_lead_source</t>
+  </si>
+  <si>
+    <t>job_lead_source_type</t>
+  </si>
+  <si>
+    <t>salesperson</t>
+  </si>
+  <si>
+    <t>call_date</t>
+  </si>
+  <si>
+    <t>call_time</t>
+  </si>
+  <si>
+    <t>timestamps</t>
+  </si>
+  <si>
+    <t>unique location identifier</t>
+  </si>
+  <si>
+    <t>date call was scheduled</t>
+  </si>
+  <si>
+    <t>marketing lead source for customer (level 1 depth, ex. "radio")</t>
+  </si>
+  <si>
+    <t>marketing lead source customer (level 2 depth, ex. "radio for discounted tune-up in 2017")</t>
+  </si>
+  <si>
+    <t>date of appointment</t>
+  </si>
+  <si>
+    <t>category of estimate (furnace, water heater, etc.)</t>
+  </si>
+  <si>
+    <t>marketing lead source for particular sales call (level 1 depth, ex. "technician")</t>
+  </si>
+  <si>
+    <t>marketing lead source particular sales call (level 2 depth, ex. "technician- Jairo")</t>
+  </si>
+  <si>
+    <t>time of appointment</t>
+  </si>
+  <si>
+    <t>job_no</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>job_class</t>
+  </si>
+  <si>
+    <t>job_type</t>
+  </si>
+  <si>
+    <t>dept</t>
+  </si>
+  <si>
+    <t>unique job identifier; secondary key</t>
+  </si>
+  <si>
+    <t>date job ended</t>
+  </si>
+  <si>
+    <t>class of job (water heater install, etc.)</t>
+  </si>
+  <si>
+    <t>type of job (water heater install, etc.)</t>
+  </si>
+  <si>
+    <t>department- install, service, maintenance, etc.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +513,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +630,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -563,7 +641,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -573,24 +651,238 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="97.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="83.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>